<commit_message>
Correção na tabela de dados
</commit_message>
<xml_diff>
--- a/docs/Tabelas de dados.xlsx
+++ b/docs/Tabelas de dados.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27813"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4884913A-417A-4F0C-82E3-FFC6D110B5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{942D1158-EF89-44AE-82E2-D983BDF8675B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11384,6 +11384,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>DuraçãoMédia(ms)</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -12214,6 +12217,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>MédiadoValorTotaldasSoluções</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -13044,6 +13050,9 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>MédiadaEnergiaTotaldasSoluções</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -23891,7 +23900,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="28" name="Gráfico 6">
+        <xdr:cNvPr id="7" name="Gráfico 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEA7E667-D1DD-9DD7-F2F2-19CAC2127EB3}"/>
@@ -23930,7 +23939,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="76" name="Gráfico 7">
+        <xdr:cNvPr id="8" name="Gráfico 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8736BAC5-661E-F4DE-6E70-F20B7D5F0E10}"/>
@@ -23969,7 +23978,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="64" name="Gráfico 8">
+        <xdr:cNvPr id="38" name="Gráfico 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62A3ACE2-29A3-53FB-4A00-6CCFFE0AF1D7}"/>
@@ -24008,7 +24017,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="68" name="Gráfico 11">
+        <xdr:cNvPr id="12" name="Gráfico 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B93E522D-2BA2-3507-6759-91C9EE2E4C3C}"/>
@@ -24047,7 +24056,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="51" name="Gráfico 12">
+        <xdr:cNvPr id="13" name="Gráfico 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC7CBF43-40DE-A4E4-E4BE-B5ECE039339C}"/>
@@ -24086,7 +24095,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="82" name="Gráfico 22">
+        <xdr:cNvPr id="23" name="Gráfico 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C66888D4-AF7E-EAC4-BDFA-CC4BD4614CDB}"/>
@@ -24125,7 +24134,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="96" name="Gráfico 25">
+        <xdr:cNvPr id="26" name="Gráfico 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3DBBB47-F74B-9A95-9223-A164D1B4537F}"/>
@@ -24164,7 +24173,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="95" name="Gráfico 26">
+        <xdr:cNvPr id="27" name="Gráfico 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4266CC4-2B09-F33E-6E1E-AC69347D7D5A}"/>
@@ -24510,7 +24519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B19:AT279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
@@ -24540,7 +24549,6 @@
     <col min="40" max="40" width="23" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="23.85546875" customWidth="1"/>
     <col min="42" max="42" width="25" bestFit="1" customWidth="1"/>
-    <col min="47" max="50" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="19" spans="2:42">
@@ -35997,7 +36005,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N20:S279">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N19:S279">
     <sortCondition ref="S20:S279"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>